<commit_message>
changes on library file
</commit_message>
<xml_diff>
--- a/Library/SmokeSanityTestCases.xlsx
+++ b/Library/SmokeSanityTestCases.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\Automation\AutomationTest\Library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QA\AutomationTest\Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="26328" yWindow="0" windowWidth="13908" windowHeight="12300"/>
+    <workbookView xWindow="26325" yWindow="0" windowWidth="13905" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -162,7 +162,7 @@
     <t>OnHold: LPH</t>
   </si>
   <si>
-    <t>Laboratory\TC006GenerateLabReport(OP).py</t>
+    <t>Laboratory\TC005GenerateLabReport.py</t>
   </si>
 </sst>
 </file>
@@ -522,19 +522,19 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.5546875" customWidth="1"/>
+    <col min="1" max="1" width="54.5703125" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.33203125" customWidth="1"/>
+    <col min="3" max="4" width="11.28515625" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -557,7 +557,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -576,7 +576,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>42</v>
       </c>
@@ -595,7 +595,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
@@ -614,7 +614,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -633,7 +633,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -652,7 +652,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -674,7 +674,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -693,7 +693,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -712,7 +712,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -731,7 +731,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -750,7 +750,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -769,7 +769,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>43</v>
       </c>
@@ -790,7 +790,7 @@
       </c>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -811,7 +811,7 @@
       </c>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -832,7 +832,7 @@
       </c>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
@@ -853,7 +853,7 @@
       </c>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
@@ -874,7 +874,7 @@
       </c>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
updated OPD billing test script
</commit_message>
<xml_diff>
--- a/Library/SmokeSanityTestCases.xlsx
+++ b/Library/SmokeSanityTestCases.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QA\AutomationTest\Library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\Automation\AutomationTest\Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="26325" yWindow="0" windowWidth="13905" windowHeight="12300"/>
+    <workbookView xWindow="27264" yWindow="0" windowWidth="13908" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -90,9 +90,6 @@
     <t>TC012</t>
   </si>
   <si>
-    <t>Norun</t>
-  </si>
-  <si>
     <t>Run No.</t>
   </si>
   <si>
@@ -136,6 +133,9 @@
   </si>
   <si>
     <t>TC002</t>
+  </si>
+  <si>
+    <t>NoRun</t>
   </si>
 </sst>
 </file>
@@ -499,19 +499,19 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="54.5703125" customWidth="1"/>
+    <col min="1" max="1" width="54.5546875" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.28515625" customWidth="1"/>
+    <col min="3" max="4" width="11.33203125" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -522,7 +522,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -531,15 +531,15 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -553,12 +553,12 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
@@ -567,17 +567,17 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -591,12 +591,12 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>23</v>
+      <c r="B5" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
@@ -610,12 +610,12 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>31</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
@@ -629,12 +629,12 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>32</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>6</v>
@@ -648,12 +648,12 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>23</v>
+      <c r="B8" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>6</v>
@@ -667,15 +667,15 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="J8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>23</v>
+        <v>33</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>14</v>
@@ -689,12 +689,12 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>23</v>
+        <v>34</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>14</v>
@@ -708,12 +708,12 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>23</v>
+      <c r="B11" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>14</v>
@@ -727,12 +727,12 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>14</v>
@@ -746,12 +746,12 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>23</v>
+      <c r="B13" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>14</v>
@@ -765,12 +765,12 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>14</v>
@@ -779,17 +779,17 @@
         <v>0</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>14</v>
@@ -798,7 +798,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>

</xml_diff>